<commit_message>
Finalizado el desarrollo del termometro
</commit_message>
<xml_diff>
--- a/bizapps-sevadu/WebContent/public/plantilla.xlsx
+++ b/bizapps-sevadu/WebContent/public/plantilla.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>DIAS RECORRIDOS</t>
   </si>
@@ -27,12 +27,6 @@
     <t>D/HABIL FALTANTE</t>
   </si>
   <si>
-    <t>15-07-2014 / Rango Fechas:2014-07-01 al 2014-07-15</t>
-  </si>
-  <si>
-    <t>IBERO AMERICANA LICORES, C.A. (IALCA) (2014)</t>
-  </si>
-  <si>
     <t>MES</t>
   </si>
   <si>
@@ -45,9 +39,6 @@
     <t>Cj diarias</t>
   </si>
   <si>
-    <t>Proyeccìon</t>
-  </si>
-  <si>
     <t>ZONA</t>
   </si>
   <si>
@@ -76,6 +67,9 @@
   </si>
   <si>
     <t xml:space="preserve"> para alcanzar meta</t>
+  </si>
+  <si>
+    <t>Proyección</t>
   </si>
 </sst>
 </file>
@@ -438,6 +432,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -464,9 +461,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -765,7 +759,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -779,6 +773,8 @@
     <col min="8" max="8" width="15.140625" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="32.25" thickBot="1">
@@ -795,73 +791,69 @@
       <c r="G1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7"/>
       <c r="G2" s="8"/>
       <c r="H2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="27"/>
+      <c r="K2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="1:12" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="E3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="F3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="G3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="I3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="J3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="28"/>
-      <c r="L3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="30"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" thickTop="1"/>
   </sheetData>

</xml_diff>